<commit_message>
Updated permissions query script
</commit_message>
<xml_diff>
--- a/DB_Exemplo_Permissoes/Tabelas Permissoes.xlsx
+++ b/DB_Exemplo_Permissoes/Tabelas Permissoes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Administradores" sheetId="5" r:id="rId1"/>
@@ -92,7 +92,7 @@
     <t>É melhor cada Investigador ter permissão de update ao valor limite das suas culturas, caso contrario, teria de se contactar um administrador para o efeito, não valendo a pena</t>
   </si>
   <si>
-    <t>SPs para selects e updates à coluna aos limites da tabela DBA.Culturas. Apenas pode ver as culturas que apontam para o seu idInvestigador correspondente</t>
+    <t>SPs/Triggers para selects e updates à coluna aos limites da tabela DBA.Culturas. Apenas pode ver as culturas que apontam para o seu idInvestigador correspondente</t>
   </si>
 </sst>
 </file>
@@ -773,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,7 +935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>